<commit_message>
Thêm dữ liệu huyện xã phường
</commit_message>
<xml_diff>
--- a/ldtiep.docs/Cấu trúc bảng.xlsx
+++ b/ldtiep.docs/Cấu trúc bảng.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\do-an\ldtiep.docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D4DE89A1-971F-442F-A615-8E940E2C8E41}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{876796E6-D434-46ED-9555-0509C2DAB358}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1275" yWindow="795" windowWidth="24210" windowHeight="11295" xr2:uid="{2010E0CC-8981-4F39-BFC2-E9E2B2601EEF}"/>
+    <workbookView xWindow="420" yWindow="2160" windowWidth="24210" windowHeight="11295" xr2:uid="{2010E0CC-8981-4F39-BFC2-E9E2B2601EEF}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -20,22 +20,12 @@
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
-    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
-      <xcalcf:calcFeatures>
-        <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:Single"/>
-        <xcalcf:feature name="microsoft.com:FV"/>
-        <xcalcf:feature name="microsoft.com:CNMTM"/>
-        <xcalcf:feature name="microsoft.com:LET_WF"/>
-        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
-      </xcalcf:calcFeatures>
-    </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="78" uniqueCount="71">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="103" uniqueCount="92">
   <si>
     <t>Bảng lưu màu sắc</t>
   </si>
@@ -58,12 +48,6 @@
     <t>ProductID</t>
   </si>
   <si>
-    <t>Mã sản phẩm</t>
-  </si>
-  <si>
-    <t>Tên SP</t>
-  </si>
-  <si>
     <t>ProductCode</t>
   </si>
   <si>
@@ -248,13 +232,82 @@
   </si>
   <si>
     <t>Phường / xã</t>
+  </si>
+  <si>
+    <t>DistrictID</t>
+  </si>
+  <si>
+    <t>Mã huyện</t>
+  </si>
+  <si>
+    <t>Name</t>
+  </si>
+  <si>
+    <t>CommuneID</t>
+  </si>
+  <si>
+    <t>Tên</t>
+  </si>
+  <si>
+    <t>Mã xã</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Tên xã </t>
+  </si>
+  <si>
+    <t>Xã huyện</t>
+  </si>
+  <si>
+    <t>CityID</t>
+  </si>
+  <si>
+    <t>Mã thành phố</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Mã thành phố </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Tên thành phố </t>
+  </si>
+  <si>
+    <t>ldt_order</t>
+  </si>
+  <si>
+    <t>ldt_district</t>
+  </si>
+  <si>
+    <t>ldt_commune</t>
+  </si>
+  <si>
+    <t>ldt_city</t>
+  </si>
+  <si>
+    <t>ldt_product</t>
+  </si>
+  <si>
+    <t>ldt_color</t>
+  </si>
+  <si>
+    <t>ldt_category</t>
+  </si>
+  <si>
+    <t>ldt_size</t>
+  </si>
+  <si>
+    <t>ldt_payment</t>
+  </si>
+  <si>
+    <t>Mã SP</t>
+  </si>
+  <si>
+    <t>ID sản phẩm</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -268,6 +321,14 @@
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <charset val="163"/>
       <scheme val="minor"/>
     </font>
   </fonts>
@@ -348,20 +409,21 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="2" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -676,21 +738,21 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F93C9DBF-709E-4039-B299-89A574944C00}">
-  <dimension ref="A3:Q20"/>
+  <dimension ref="A3:Q22"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G17" sqref="G17"/>
+      <selection activeCell="D11" sqref="D11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="13.42578125" customWidth="1"/>
-    <col min="2" max="2" width="15.85546875" customWidth="1"/>
+    <col min="1" max="1" width="27.7109375" customWidth="1"/>
+    <col min="2" max="2" width="25.7109375" customWidth="1"/>
     <col min="4" max="5" width="14.42578125" customWidth="1"/>
     <col min="6" max="6" width="21.140625" customWidth="1"/>
     <col min="7" max="7" width="15.5703125" customWidth="1"/>
     <col min="8" max="8" width="14.42578125" customWidth="1"/>
-    <col min="9" max="9" width="12.28515625" customWidth="1"/>
+    <col min="9" max="9" width="14.7109375" customWidth="1"/>
     <col min="10" max="10" width="19.7109375" customWidth="1"/>
     <col min="11" max="11" width="20.28515625" customWidth="1"/>
     <col min="12" max="12" width="21.7109375" customWidth="1"/>
@@ -705,9 +767,14 @@
       <c r="A3" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="B3" s="3"/>
-      <c r="D3" s="8" t="s">
+      <c r="B3" s="10" t="s">
+        <v>86</v>
+      </c>
+      <c r="D3" s="6" t="s">
         <v>5</v>
+      </c>
+      <c r="E3" s="9" t="s">
+        <v>85</v>
       </c>
     </row>
     <row r="4" spans="1:17" x14ac:dyDescent="0.25">
@@ -718,40 +785,40 @@
         <v>2</v>
       </c>
       <c r="D4" s="1" t="s">
-        <v>7</v>
+        <v>91</v>
       </c>
       <c r="E4" s="1" t="s">
-        <v>8</v>
+        <v>90</v>
       </c>
       <c r="F4" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="G4" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="G4" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="H4" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="I4" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="J4" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="K4" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="L4" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="M4" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="N4" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="H4" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="I4" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="J4" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="K4" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="L4" s="1" t="s">
-        <v>32</v>
-      </c>
-      <c r="M4" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="N4" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="O4" s="4" t="s">
-        <v>27</v>
+      <c r="O4" s="1" t="s">
+        <v>25</v>
       </c>
     </row>
     <row r="5" spans="1:17" x14ac:dyDescent="0.25">
@@ -765,208 +832,280 @@
         <v>6</v>
       </c>
       <c r="E5" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="F5" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="F5" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="G5" s="4" t="s">
-        <v>25</v>
+      <c r="G5" s="1" t="s">
+        <v>23</v>
       </c>
       <c r="H5" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="I5" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="I5" s="1" t="s">
-        <v>16</v>
-      </c>
       <c r="J5" s="1" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="K5" s="1" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="L5" s="1" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="M5" s="1" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="N5" s="1" t="s">
-        <v>28</v>
-      </c>
-      <c r="O5" s="4" t="s">
-        <v>29</v>
+        <v>26</v>
+      </c>
+      <c r="O5" s="1" t="s">
+        <v>27</v>
       </c>
     </row>
     <row r="6" spans="1:17" x14ac:dyDescent="0.25">
       <c r="D6" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
     </row>
     <row r="7" spans="1:17" x14ac:dyDescent="0.25">
       <c r="F7" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
     </row>
     <row r="8" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A8" s="6" t="s">
-        <v>22</v>
+      <c r="A8" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="B8" s="9" t="s">
+        <v>87</v>
       </c>
     </row>
     <row r="9" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="B9" s="4" t="s">
-        <v>27</v>
+        <v>24</v>
+      </c>
+      <c r="B9" s="1" t="s">
+        <v>25</v>
       </c>
     </row>
     <row r="10" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
-        <v>30</v>
-      </c>
-      <c r="B10" s="4" t="s">
-        <v>31</v>
-      </c>
-      <c r="E10" s="7" t="s">
+        <v>28</v>
+      </c>
+      <c r="B10" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="E10" s="5" t="s">
+        <v>36</v>
+      </c>
+      <c r="F10" s="9" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="11" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="E11" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="F11" s="1" t="s">
         <v>38</v>
       </c>
-    </row>
-    <row r="11" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="E11" t="s">
+      <c r="G11" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="H11" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="I11" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="J11" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="K11" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="L11" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="M11" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="N11" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="O11" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="P11" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="Q11" s="1" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="12" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A12" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="B12" s="9" t="s">
+        <v>88</v>
+      </c>
+      <c r="E12" s="1" t="s">
         <v>39</v>
       </c>
-      <c r="F11" t="s">
+      <c r="F12" s="1" t="s">
         <v>40</v>
       </c>
-      <c r="G11" t="s">
-        <v>43</v>
-      </c>
-      <c r="H11" t="s">
-        <v>45</v>
-      </c>
-      <c r="I11" t="s">
-        <v>47</v>
-      </c>
-      <c r="J11" t="s">
-        <v>49</v>
-      </c>
-      <c r="K11" t="s">
-        <v>51</v>
-      </c>
-      <c r="L11" t="s">
-        <v>54</v>
-      </c>
-      <c r="M11" t="s">
-        <v>56</v>
-      </c>
-      <c r="N11" t="s">
+      <c r="G12" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="H12" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="I12" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="J12" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="K12" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="L12" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="M12" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="N12" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="O12" s="1" t="s">
         <v>58</v>
       </c>
-      <c r="O11" t="s">
+      <c r="P12" s="1" t="s">
         <v>61</v>
       </c>
-      <c r="P11" t="s">
-        <v>62</v>
-      </c>
-      <c r="Q11" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="12" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A12" s="5" t="s">
-        <v>21</v>
-      </c>
-      <c r="E12" t="s">
-        <v>41</v>
-      </c>
-      <c r="F12" t="s">
-        <v>42</v>
-      </c>
-      <c r="G12" t="s">
-        <v>44</v>
-      </c>
-      <c r="H12" t="s">
-        <v>46</v>
-      </c>
-      <c r="I12" t="s">
-        <v>48</v>
-      </c>
-      <c r="J12" t="s">
-        <v>50</v>
-      </c>
-      <c r="K12" t="s">
-        <v>52</v>
-      </c>
-      <c r="L12" t="s">
-        <v>55</v>
-      </c>
-      <c r="M12" t="s">
-        <v>57</v>
-      </c>
-      <c r="N12" t="s">
-        <v>59</v>
-      </c>
-      <c r="O12" t="s">
-        <v>60</v>
-      </c>
-      <c r="P12" t="s">
+      <c r="Q12" s="1" t="s">
         <v>63</v>
-      </c>
-      <c r="Q12" t="s">
-        <v>65</v>
       </c>
     </row>
     <row r="13" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A13" s="1" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="K13" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
     </row>
     <row r="14" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A14" s="1" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
     </row>
     <row r="16" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A16" s="9" t="s">
+      <c r="A16" s="7" t="s">
+        <v>60</v>
+      </c>
+      <c r="B16" s="11" t="s">
+        <v>89</v>
+      </c>
+      <c r="E16" s="8" t="s">
+        <v>67</v>
+      </c>
+      <c r="F16" s="9" t="s">
+        <v>82</v>
+      </c>
+      <c r="I16" s="8" t="s">
+        <v>66</v>
+      </c>
+      <c r="J16" s="9" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="17" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A17" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="B17" s="1" t="s">
         <v>62</v>
       </c>
-      <c r="B16" s="9"/>
-      <c r="E16" s="10" t="s">
+      <c r="E17" s="1" t="s">
+        <v>70</v>
+      </c>
+      <c r="F17" s="1" t="s">
+        <v>73</v>
+      </c>
+      <c r="G17" s="1" t="s">
+        <v>78</v>
+      </c>
+      <c r="I17" s="1" t="s">
+        <v>79</v>
+      </c>
+      <c r="J17" s="1" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="18" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A18" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="B18" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="E18" s="1" t="s">
         <v>69</v>
       </c>
-      <c r="H16" s="10" t="s">
+      <c r="F18" s="1" t="s">
+        <v>71</v>
+      </c>
+      <c r="G18" s="1" t="s">
+        <v>77</v>
+      </c>
+      <c r="I18" s="1" t="s">
+        <v>77</v>
+      </c>
+      <c r="J18" s="1" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="20" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="E20" s="8" t="s">
         <v>68</v>
       </c>
-    </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A17" s="1" t="s">
-        <v>67</v>
-      </c>
-      <c r="B17" s="1" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A18" s="1" t="s">
-        <v>66</v>
-      </c>
-      <c r="B18" s="1" t="s">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="E20" s="10" t="s">
-        <v>70</v>
+      <c r="F20" s="9" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="21" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="E21" s="1" t="s">
+        <v>74</v>
+      </c>
+      <c r="F21" s="1" t="s">
+        <v>75</v>
+      </c>
+      <c r="G21" s="1" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="22" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="E22" s="1" t="s">
+        <v>72</v>
+      </c>
+      <c r="F22" s="1" t="s">
+        <v>71</v>
+      </c>
+      <c r="G22" s="1" t="s">
+        <v>69</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Thêm api thêm màu, sửa màu, lấy danh sách màu
</commit_message>
<xml_diff>
--- a/ldtiep.docs/Cấu trúc bảng.xlsx
+++ b/ldtiep.docs/Cấu trúc bảng.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\do-an\ldtiep.docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{876796E6-D434-46ED-9555-0509C2DAB358}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2BED389D-E33B-4EFB-889B-01FCA5A5DF53}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="420" yWindow="2160" windowWidth="24210" windowHeight="11295" xr2:uid="{2010E0CC-8981-4F39-BFC2-E9E2B2601EEF}"/>
+    <workbookView xWindow="2760" yWindow="1065" windowWidth="24210" windowHeight="11295" xr2:uid="{2010E0CC-8981-4F39-BFC2-E9E2B2601EEF}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -741,7 +741,7 @@
   <dimension ref="A3:Q22"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D11" sqref="D11"/>
+      <selection activeCell="G15" sqref="G15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
vẽ form thêm thể loại và phân tích lại bảng
</commit_message>
<xml_diff>
--- a/ldtiep.docs/Cấu trúc bảng.xlsx
+++ b/ldtiep.docs/Cấu trúc bảng.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\do-an\ldtiep.docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2BED389D-E33B-4EFB-889B-01FCA5A5DF53}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{93F3CBE1-FD44-4DE7-ACEA-585656FD6AB4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2760" yWindow="1065" windowWidth="24210" windowHeight="11295" xr2:uid="{2010E0CC-8981-4F39-BFC2-E9E2B2601EEF}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{2010E0CC-8981-4F39-BFC2-E9E2B2601EEF}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="103" uniqueCount="92">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="110" uniqueCount="98">
   <si>
     <t>Bảng lưu màu sắc</t>
   </si>
@@ -301,6 +301,24 @@
   </si>
   <si>
     <t>ID sản phẩm</t>
+  </si>
+  <si>
+    <t>Mã thể loại cha</t>
+  </si>
+  <si>
+    <t>ParentID</t>
+  </si>
+  <si>
+    <t>Thứ tự sắp xếp</t>
+  </si>
+  <si>
+    <t>SortOrder</t>
+  </si>
+  <si>
+    <t>CategoryType</t>
+  </si>
+  <si>
+    <t>Nam;Nữ;Trẻ em</t>
   </si>
 </sst>
 </file>
@@ -738,16 +756,17 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F93C9DBF-709E-4039-B299-89A574944C00}">
-  <dimension ref="A3:Q22"/>
+  <dimension ref="A3:Q27"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G15" sqref="G15"/>
+      <selection activeCell="F14" sqref="F14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="27.7109375" customWidth="1"/>
     <col min="2" max="2" width="25.7109375" customWidth="1"/>
+    <col min="3" max="3" width="17.140625" customWidth="1"/>
     <col min="4" max="5" width="14.42578125" customWidth="1"/>
     <col min="6" max="6" width="21.140625" customWidth="1"/>
     <col min="7" max="7" width="15.5703125" customWidth="1"/>
@@ -890,6 +909,15 @@
       <c r="B9" s="1" t="s">
         <v>25</v>
       </c>
+      <c r="C9" s="1" t="s">
+        <v>92</v>
+      </c>
+      <c r="D9" s="1" t="s">
+        <v>94</v>
+      </c>
+      <c r="E9" s="1" t="s">
+        <v>20</v>
+      </c>
     </row>
     <row r="10" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
@@ -898,52 +926,19 @@
       <c r="B10" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="E10" s="5" t="s">
-        <v>36</v>
-      </c>
-      <c r="F10" s="9" t="s">
-        <v>81</v>
+      <c r="C10" s="1" t="s">
+        <v>93</v>
+      </c>
+      <c r="D10" s="1" t="s">
+        <v>95</v>
+      </c>
+      <c r="E10" s="1" t="s">
+        <v>96</v>
       </c>
     </row>
     <row r="11" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="E11" s="1" t="s">
-        <v>37</v>
-      </c>
-      <c r="F11" s="1" t="s">
-        <v>38</v>
-      </c>
-      <c r="G11" s="1" t="s">
-        <v>41</v>
-      </c>
-      <c r="H11" s="1" t="s">
-        <v>43</v>
-      </c>
-      <c r="I11" s="1" t="s">
-        <v>45</v>
-      </c>
-      <c r="J11" s="1" t="s">
-        <v>47</v>
-      </c>
-      <c r="K11" s="1" t="s">
-        <v>49</v>
-      </c>
-      <c r="L11" s="1" t="s">
-        <v>52</v>
-      </c>
-      <c r="M11" s="1" t="s">
-        <v>54</v>
-      </c>
-      <c r="N11" s="1" t="s">
-        <v>56</v>
-      </c>
-      <c r="O11" s="1" t="s">
-        <v>59</v>
-      </c>
-      <c r="P11" s="1" t="s">
-        <v>60</v>
-      </c>
-      <c r="Q11" s="1" t="s">
-        <v>62</v>
+      <c r="E11" t="s">
+        <v>97</v>
       </c>
     </row>
     <row r="12" spans="1:17" x14ac:dyDescent="0.25">
@@ -953,45 +948,6 @@
       <c r="B12" s="9" t="s">
         <v>88</v>
       </c>
-      <c r="E12" s="1" t="s">
-        <v>39</v>
-      </c>
-      <c r="F12" s="1" t="s">
-        <v>40</v>
-      </c>
-      <c r="G12" s="1" t="s">
-        <v>42</v>
-      </c>
-      <c r="H12" s="1" t="s">
-        <v>44</v>
-      </c>
-      <c r="I12" s="1" t="s">
-        <v>46</v>
-      </c>
-      <c r="J12" s="1" t="s">
-        <v>48</v>
-      </c>
-      <c r="K12" s="1" t="s">
-        <v>50</v>
-      </c>
-      <c r="L12" s="1" t="s">
-        <v>53</v>
-      </c>
-      <c r="M12" s="1" t="s">
-        <v>55</v>
-      </c>
-      <c r="N12" s="1" t="s">
-        <v>57</v>
-      </c>
-      <c r="O12" s="1" t="s">
-        <v>58</v>
-      </c>
-      <c r="P12" s="1" t="s">
-        <v>61</v>
-      </c>
-      <c r="Q12" s="1" t="s">
-        <v>63</v>
-      </c>
     </row>
     <row r="13" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A13" s="1" t="s">
@@ -1000,9 +956,6 @@
       <c r="B13" s="1" t="s">
         <v>31</v>
       </c>
-      <c r="K13" t="s">
-        <v>51</v>
-      </c>
     </row>
     <row r="14" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A14" s="1" t="s">
@@ -1012,6 +965,14 @@
         <v>35</v>
       </c>
     </row>
+    <row r="15" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="E15" s="5" t="s">
+        <v>36</v>
+      </c>
+      <c r="F15" s="9" t="s">
+        <v>81</v>
+      </c>
+    </row>
     <row r="16" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A16" s="7" t="s">
         <v>60</v>
@@ -1019,20 +980,47 @@
       <c r="B16" s="11" t="s">
         <v>89</v>
       </c>
-      <c r="E16" s="8" t="s">
-        <v>67</v>
-      </c>
-      <c r="F16" s="9" t="s">
-        <v>82</v>
-      </c>
-      <c r="I16" s="8" t="s">
-        <v>66</v>
-      </c>
-      <c r="J16" s="9" t="s">
-        <v>84</v>
-      </c>
-    </row>
-    <row r="17" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="E16" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="F16" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="G16" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="H16" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="I16" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="J16" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="K16" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="L16" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="M16" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="N16" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="O16" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="P16" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="Q16" s="1" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="17" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A17" s="1" t="s">
         <v>65</v>
       </c>
@@ -1040,71 +1028,131 @@
         <v>62</v>
       </c>
       <c r="E17" s="1" t="s">
-        <v>70</v>
+        <v>39</v>
       </c>
       <c r="F17" s="1" t="s">
-        <v>73</v>
+        <v>40</v>
       </c>
       <c r="G17" s="1" t="s">
-        <v>78</v>
+        <v>42</v>
+      </c>
+      <c r="H17" s="1" t="s">
+        <v>44</v>
       </c>
       <c r="I17" s="1" t="s">
-        <v>79</v>
+        <v>46</v>
       </c>
       <c r="J17" s="1" t="s">
-        <v>80</v>
-      </c>
-    </row>
-    <row r="18" spans="1:10" x14ac:dyDescent="0.25">
+        <v>48</v>
+      </c>
+      <c r="K17" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="L17" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="M17" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="N17" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="O17" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="P17" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="Q17" s="1" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="18" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A18" s="1" t="s">
         <v>64</v>
       </c>
       <c r="B18" s="1" t="s">
         <v>63</v>
       </c>
-      <c r="E18" s="1" t="s">
+      <c r="K18" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="21" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="E21" s="8" t="s">
+        <v>67</v>
+      </c>
+      <c r="F21" s="9" t="s">
+        <v>82</v>
+      </c>
+      <c r="I21" s="8" t="s">
+        <v>66</v>
+      </c>
+      <c r="J21" s="9" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="22" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="E22" s="1" t="s">
+        <v>70</v>
+      </c>
+      <c r="F22" s="1" t="s">
+        <v>73</v>
+      </c>
+      <c r="G22" s="1" t="s">
+        <v>78</v>
+      </c>
+      <c r="I22" s="1" t="s">
+        <v>79</v>
+      </c>
+      <c r="J22" s="1" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="23" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="E23" s="1" t="s">
         <v>69</v>
       </c>
-      <c r="F18" s="1" t="s">
+      <c r="F23" s="1" t="s">
         <v>71</v>
       </c>
-      <c r="G18" s="1" t="s">
+      <c r="G23" s="1" t="s">
         <v>77</v>
       </c>
-      <c r="I18" s="1" t="s">
+      <c r="I23" s="1" t="s">
         <v>77</v>
       </c>
-      <c r="J18" s="1" t="s">
+      <c r="J23" s="1" t="s">
         <v>71</v>
       </c>
     </row>
-    <row r="20" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="E20" s="8" t="s">
+    <row r="25" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="E25" s="8" t="s">
         <v>68</v>
       </c>
-      <c r="F20" s="9" t="s">
+      <c r="F25" s="9" t="s">
         <v>83</v>
       </c>
     </row>
-    <row r="21" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="E21" s="1" t="s">
+    <row r="26" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="E26" s="1" t="s">
         <v>74</v>
       </c>
-      <c r="F21" s="1" t="s">
+      <c r="F26" s="1" t="s">
         <v>75</v>
       </c>
-      <c r="G21" s="1" t="s">
+      <c r="G26" s="1" t="s">
         <v>76</v>
       </c>
     </row>
-    <row r="22" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="E22" s="1" t="s">
+    <row r="27" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="E27" s="1" t="s">
         <v>72</v>
       </c>
-      <c r="F22" s="1" t="s">
+      <c r="F27" s="1" t="s">
         <v>71</v>
       </c>
-      <c r="G22" s="1" t="s">
+      <c r="G27" s="1" t="s">
         <v>69</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Thêm chọn thể loại, màu sắc vào form thêm sản phẩm
</commit_message>
<xml_diff>
--- a/ldtiep.docs/Cấu trúc bảng.xlsx
+++ b/ldtiep.docs/Cấu trúc bảng.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\do-an\ldtiep.docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{93F3CBE1-FD44-4DE7-ACEA-585656FD6AB4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6D027736-900A-42EF-A2FD-E7A74795FFE3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{2010E0CC-8981-4F39-BFC2-E9E2B2601EEF}"/>
   </bookViews>
@@ -759,7 +759,7 @@
   <dimension ref="A3:Q27"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F14" sqref="F14"/>
+      <selection activeCell="H12" sqref="H12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
Hoàn thiện giao diện form thêm sản phẩm
</commit_message>
<xml_diff>
--- a/ldtiep.docs/Cấu trúc bảng.xlsx
+++ b/ldtiep.docs/Cấu trúc bảng.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\do-an\ldtiep.docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6D027736-900A-42EF-A2FD-E7A74795FFE3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{14C13218-2995-49B5-8790-7EE9F8277345}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{2010E0CC-8981-4F39-BFC2-E9E2B2601EEF}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="110" uniqueCount="98">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="182" uniqueCount="106">
   <si>
     <t>Bảng lưu màu sắc</t>
   </si>
@@ -319,6 +319,30 @@
   </si>
   <si>
     <t>Nam;Nữ;Trẻ em</t>
+  </si>
+  <si>
+    <t>CreatedDate</t>
+  </si>
+  <si>
+    <t>Ngày tạo</t>
+  </si>
+  <si>
+    <t>Người tạo</t>
+  </si>
+  <si>
+    <t>CreatedBy</t>
+  </si>
+  <si>
+    <t>Ngày sửa</t>
+  </si>
+  <si>
+    <t>ModifiedDate</t>
+  </si>
+  <si>
+    <t>ModifiedBy</t>
+  </si>
+  <si>
+    <t>Người sửa</t>
   </si>
 </sst>
 </file>
@@ -756,10 +780,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F93C9DBF-709E-4039-B299-89A574944C00}">
-  <dimension ref="A3:Q27"/>
+  <dimension ref="A3:Q43"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H12" sqref="H12"/>
+      <selection activeCell="C4" sqref="C4:F5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -775,126 +799,62 @@
     <col min="10" max="10" width="19.7109375" customWidth="1"/>
     <col min="11" max="11" width="20.28515625" customWidth="1"/>
     <col min="12" max="12" width="21.7109375" customWidth="1"/>
-    <col min="13" max="13" width="17.28515625" customWidth="1"/>
+    <col min="13" max="13" width="28.7109375" customWidth="1"/>
     <col min="14" max="14" width="23.140625" customWidth="1"/>
     <col min="15" max="15" width="15.85546875" customWidth="1"/>
     <col min="16" max="16" width="22.7109375" customWidth="1"/>
     <col min="17" max="17" width="27.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="3" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
         <v>0</v>
       </c>
       <c r="B3" s="10" t="s">
         <v>86</v>
       </c>
-      <c r="D3" s="6" t="s">
-        <v>5</v>
-      </c>
-      <c r="E3" s="9" t="s">
-        <v>85</v>
-      </c>
-    </row>
-    <row r="4" spans="1:17" x14ac:dyDescent="0.25">
+    </row>
+    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
         <v>1</v>
       </c>
       <c r="B4" s="1" t="s">
         <v>2</v>
       </c>
+      <c r="C4" s="1" t="s">
+        <v>99</v>
+      </c>
       <c r="D4" s="1" t="s">
-        <v>91</v>
+        <v>100</v>
       </c>
       <c r="E4" s="1" t="s">
-        <v>90</v>
+        <v>102</v>
       </c>
       <c r="F4" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="G4" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="H4" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="I4" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="J4" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="K4" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="L4" s="1" t="s">
-        <v>30</v>
-      </c>
-      <c r="M4" s="1" t="s">
-        <v>31</v>
-      </c>
-      <c r="N4" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="O4" s="1" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="5" spans="1:17" x14ac:dyDescent="0.25">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
         <v>3</v>
       </c>
       <c r="B5" s="1" t="s">
         <v>4</v>
       </c>
+      <c r="C5" s="1" t="s">
+        <v>98</v>
+      </c>
       <c r="D5" s="1" t="s">
-        <v>6</v>
+        <v>101</v>
       </c>
       <c r="E5" s="1" t="s">
-        <v>7</v>
+        <v>103</v>
       </c>
       <c r="F5" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="G5" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="H5" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="I5" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="J5" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="K5" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="L5" s="1" t="s">
-        <v>32</v>
-      </c>
-      <c r="M5" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="N5" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="O5" s="1" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="6" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="D6" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="7" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="F7" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="8" spans="1:17" x14ac:dyDescent="0.25">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A8" s="4" t="s">
         <v>20</v>
       </c>
@@ -902,7 +862,7 @@
         <v>87</v>
       </c>
     </row>
-    <row r="9" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
         <v>24</v>
       </c>
@@ -918,8 +878,20 @@
       <c r="E9" s="1" t="s">
         <v>20</v>
       </c>
-    </row>
-    <row r="10" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="F9" s="1" t="s">
+        <v>99</v>
+      </c>
+      <c r="G9" s="1" t="s">
+        <v>100</v>
+      </c>
+      <c r="H9" s="1" t="s">
+        <v>102</v>
+      </c>
+      <c r="I9" s="1" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
         <v>28</v>
       </c>
@@ -935,13 +907,25 @@
       <c r="E10" s="1" t="s">
         <v>96</v>
       </c>
-    </row>
-    <row r="11" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="F10" s="1" t="s">
+        <v>98</v>
+      </c>
+      <c r="G10" s="1" t="s">
+        <v>101</v>
+      </c>
+      <c r="H10" s="1" t="s">
+        <v>103</v>
+      </c>
+      <c r="I10" s="1" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
       <c r="E11" t="s">
         <v>97</v>
       </c>
     </row>
-    <row r="12" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A12" s="3" t="s">
         <v>19</v>
       </c>
@@ -949,75 +933,52 @@
         <v>88</v>
       </c>
     </row>
-    <row r="13" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A13" s="1" t="s">
         <v>30</v>
       </c>
       <c r="B13" s="1" t="s">
         <v>31</v>
       </c>
-    </row>
-    <row r="14" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="C13" s="1" t="s">
+        <v>99</v>
+      </c>
+      <c r="D13" s="1" t="s">
+        <v>100</v>
+      </c>
+      <c r="E13" s="1" t="s">
+        <v>102</v>
+      </c>
+      <c r="F13" s="1" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A14" s="1" t="s">
         <v>34</v>
       </c>
       <c r="B14" s="1" t="s">
         <v>35</v>
       </c>
-    </row>
-    <row r="15" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="E15" s="5" t="s">
-        <v>36</v>
-      </c>
-      <c r="F15" s="9" t="s">
-        <v>81</v>
-      </c>
-    </row>
-    <row r="16" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="C14" s="1" t="s">
+        <v>98</v>
+      </c>
+      <c r="D14" s="1" t="s">
+        <v>101</v>
+      </c>
+      <c r="E14" s="1" t="s">
+        <v>103</v>
+      </c>
+      <c r="F14" s="1" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="16" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A16" s="7" t="s">
         <v>60</v>
       </c>
       <c r="B16" s="11" t="s">
         <v>89</v>
-      </c>
-      <c r="E16" s="1" t="s">
-        <v>37</v>
-      </c>
-      <c r="F16" s="1" t="s">
-        <v>38</v>
-      </c>
-      <c r="G16" s="1" t="s">
-        <v>41</v>
-      </c>
-      <c r="H16" s="1" t="s">
-        <v>43</v>
-      </c>
-      <c r="I16" s="1" t="s">
-        <v>45</v>
-      </c>
-      <c r="J16" s="1" t="s">
-        <v>47</v>
-      </c>
-      <c r="K16" s="1" t="s">
-        <v>49</v>
-      </c>
-      <c r="L16" s="1" t="s">
-        <v>52</v>
-      </c>
-      <c r="M16" s="1" t="s">
-        <v>54</v>
-      </c>
-      <c r="N16" s="1" t="s">
-        <v>56</v>
-      </c>
-      <c r="O16" s="1" t="s">
-        <v>59</v>
-      </c>
-      <c r="P16" s="1" t="s">
-        <v>60</v>
-      </c>
-      <c r="Q16" s="1" t="s">
-        <v>62</v>
       </c>
     </row>
     <row r="17" spans="1:17" x14ac:dyDescent="0.25">
@@ -1027,44 +988,17 @@
       <c r="B17" s="1" t="s">
         <v>62</v>
       </c>
+      <c r="C17" s="1" t="s">
+        <v>99</v>
+      </c>
+      <c r="D17" s="1" t="s">
+        <v>100</v>
+      </c>
       <c r="E17" s="1" t="s">
-        <v>39</v>
+        <v>102</v>
       </c>
       <c r="F17" s="1" t="s">
-        <v>40</v>
-      </c>
-      <c r="G17" s="1" t="s">
-        <v>42</v>
-      </c>
-      <c r="H17" s="1" t="s">
-        <v>44</v>
-      </c>
-      <c r="I17" s="1" t="s">
-        <v>46</v>
-      </c>
-      <c r="J17" s="1" t="s">
-        <v>48</v>
-      </c>
-      <c r="K17" s="1" t="s">
-        <v>50</v>
-      </c>
-      <c r="L17" s="1" t="s">
-        <v>53</v>
-      </c>
-      <c r="M17" s="1" t="s">
-        <v>55</v>
-      </c>
-      <c r="N17" s="1" t="s">
-        <v>57</v>
-      </c>
-      <c r="O17" s="1" t="s">
-        <v>58</v>
-      </c>
-      <c r="P17" s="1" t="s">
-        <v>61</v>
-      </c>
-      <c r="Q17" s="1" t="s">
-        <v>63</v>
+        <v>105</v>
       </c>
     </row>
     <row r="18" spans="1:17" x14ac:dyDescent="0.25">
@@ -1074,86 +1008,410 @@
       <c r="B18" s="1" t="s">
         <v>63</v>
       </c>
-      <c r="K18" t="s">
+      <c r="C18" s="1" t="s">
+        <v>98</v>
+      </c>
+      <c r="D18" s="1" t="s">
+        <v>101</v>
+      </c>
+      <c r="E18" s="1" t="s">
+        <v>103</v>
+      </c>
+      <c r="F18" s="1" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="21" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A21" s="5" t="s">
+        <v>36</v>
+      </c>
+      <c r="B21" s="9" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="22" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A22" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="B22" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="C22" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="D22" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="E22" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="F22" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="G22" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="H22" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="I22" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="J22" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="K22" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="L22" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="M22" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="N22" s="1" t="s">
+        <v>99</v>
+      </c>
+      <c r="O22" s="1" t="s">
+        <v>100</v>
+      </c>
+      <c r="P22" s="1" t="s">
+        <v>102</v>
+      </c>
+      <c r="Q22" s="1" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="23" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A23" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="B23" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="C23" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="D23" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="E23" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="F23" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="G23" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="H23" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="I23" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="J23" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="K23" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="L23" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="M23" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="N23" s="1" t="s">
+        <v>98</v>
+      </c>
+      <c r="O23" s="1" t="s">
+        <v>101</v>
+      </c>
+      <c r="P23" s="1" t="s">
+        <v>103</v>
+      </c>
+      <c r="Q23" s="1" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="24" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="G24" t="s">
         <v>51</v>
       </c>
     </row>
-    <row r="21" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="E21" s="8" t="s">
+    <row r="27" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A27" s="8" t="s">
         <v>67</v>
       </c>
-      <c r="F21" s="9" t="s">
+      <c r="B27" s="9" t="s">
         <v>82</v>
       </c>
-      <c r="I21" s="8" t="s">
+    </row>
+    <row r="28" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A28" s="1" t="s">
+        <v>70</v>
+      </c>
+      <c r="B28" s="1" t="s">
+        <v>73</v>
+      </c>
+      <c r="C28" s="1" t="s">
+        <v>78</v>
+      </c>
+      <c r="D28" s="1" t="s">
+        <v>99</v>
+      </c>
+      <c r="E28" s="1" t="s">
+        <v>100</v>
+      </c>
+      <c r="F28" s="1" t="s">
+        <v>102</v>
+      </c>
+      <c r="G28" s="1" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="29" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A29" s="1" t="s">
+        <v>69</v>
+      </c>
+      <c r="B29" s="1" t="s">
+        <v>71</v>
+      </c>
+      <c r="C29" s="1" t="s">
+        <v>77</v>
+      </c>
+      <c r="D29" s="1" t="s">
+        <v>98</v>
+      </c>
+      <c r="E29" s="1" t="s">
+        <v>101</v>
+      </c>
+      <c r="F29" s="1" t="s">
+        <v>103</v>
+      </c>
+      <c r="G29" s="1" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="31" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A31" s="8" t="s">
+        <v>68</v>
+      </c>
+      <c r="B31" s="9" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="32" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A32" s="1" t="s">
+        <v>74</v>
+      </c>
+      <c r="B32" s="1" t="s">
+        <v>75</v>
+      </c>
+      <c r="C32" s="1" t="s">
+        <v>76</v>
+      </c>
+      <c r="D32" s="1" t="s">
+        <v>99</v>
+      </c>
+      <c r="E32" s="1" t="s">
+        <v>100</v>
+      </c>
+      <c r="F32" s="1" t="s">
+        <v>102</v>
+      </c>
+      <c r="G32" s="1" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="33" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A33" s="1" t="s">
+        <v>72</v>
+      </c>
+      <c r="B33" s="1" t="s">
+        <v>71</v>
+      </c>
+      <c r="C33" s="1" t="s">
+        <v>69</v>
+      </c>
+      <c r="D33" s="1" t="s">
+        <v>98</v>
+      </c>
+      <c r="E33" s="1" t="s">
+        <v>101</v>
+      </c>
+      <c r="F33" s="1" t="s">
+        <v>103</v>
+      </c>
+      <c r="G33" s="1" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="35" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A35" s="8" t="s">
         <v>66</v>
       </c>
-      <c r="J21" s="9" t="s">
+      <c r="B35" s="9" t="s">
         <v>84</v>
       </c>
     </row>
-    <row r="22" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="E22" s="1" t="s">
-        <v>70</v>
-      </c>
-      <c r="F22" s="1" t="s">
-        <v>73</v>
-      </c>
-      <c r="G22" s="1" t="s">
-        <v>78</v>
-      </c>
-      <c r="I22" s="1" t="s">
+    <row r="36" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A36" s="1" t="s">
         <v>79</v>
       </c>
-      <c r="J22" s="1" t="s">
+      <c r="B36" s="1" t="s">
         <v>80</v>
       </c>
-    </row>
-    <row r="23" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="E23" s="1" t="s">
-        <v>69</v>
-      </c>
-      <c r="F23" s="1" t="s">
+      <c r="C36" s="1" t="s">
+        <v>99</v>
+      </c>
+      <c r="D36" s="1" t="s">
+        <v>100</v>
+      </c>
+      <c r="E36" s="1" t="s">
+        <v>102</v>
+      </c>
+      <c r="F36" s="1" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="37" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A37" s="1" t="s">
+        <v>77</v>
+      </c>
+      <c r="B37" s="1" t="s">
         <v>71</v>
       </c>
-      <c r="G23" s="1" t="s">
-        <v>77</v>
-      </c>
-      <c r="I23" s="1" t="s">
-        <v>77</v>
-      </c>
-      <c r="J23" s="1" t="s">
-        <v>71</v>
-      </c>
-    </row>
-    <row r="25" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="E25" s="8" t="s">
-        <v>68</v>
-      </c>
-      <c r="F25" s="9" t="s">
-        <v>83</v>
-      </c>
-    </row>
-    <row r="26" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="E26" s="1" t="s">
-        <v>74</v>
-      </c>
-      <c r="F26" s="1" t="s">
-        <v>75</v>
-      </c>
-      <c r="G26" s="1" t="s">
-        <v>76</v>
-      </c>
-    </row>
-    <row r="27" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="E27" s="1" t="s">
-        <v>72</v>
-      </c>
-      <c r="F27" s="1" t="s">
-        <v>71</v>
-      </c>
-      <c r="G27" s="1" t="s">
-        <v>69</v>
+      <c r="C37" s="1" t="s">
+        <v>98</v>
+      </c>
+      <c r="D37" s="1" t="s">
+        <v>101</v>
+      </c>
+      <c r="E37" s="1" t="s">
+        <v>103</v>
+      </c>
+      <c r="F37" s="1" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="39" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A39" s="6" t="s">
+        <v>5</v>
+      </c>
+      <c r="B39" s="9" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="40" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A40" s="1" t="s">
+        <v>91</v>
+      </c>
+      <c r="B40" s="1" t="s">
+        <v>90</v>
+      </c>
+      <c r="C40" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="D40" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="E40" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="F40" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="G40" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="H40" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="I40" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="J40" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="K40" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="L40" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="M40" s="1" t="s">
+        <v>99</v>
+      </c>
+      <c r="N40" s="1" t="s">
+        <v>100</v>
+      </c>
+      <c r="O40" s="1" t="s">
+        <v>102</v>
+      </c>
+      <c r="P40" s="1" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="41" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A41" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="B41" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="C41" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="D41" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="E41" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="F41" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="G41" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="H41" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="I41" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="J41" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="K41" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="L41" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="M41" s="1" t="s">
+        <v>98</v>
+      </c>
+      <c r="N41" s="1" t="s">
+        <v>101</v>
+      </c>
+      <c r="O41" s="1" t="s">
+        <v>103</v>
+      </c>
+      <c r="P41" s="1" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="42" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A42" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="43" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="C43" t="s">
+        <v>10</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Thêm giao diện điền thông tin đơn hàng và lấy ra thông tin tỉnh thành, xã phường, huyện
</commit_message>
<xml_diff>
--- a/ldtiep.docs/Cấu trúc bảng.xlsx
+++ b/ldtiep.docs/Cấu trúc bảng.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\do-an\ldtiep.docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{14C13218-2995-49B5-8790-7EE9F8277345}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CF97C67D-B131-4EC6-8107-3837FB4F59F8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{2010E0CC-8981-4F39-BFC2-E9E2B2601EEF}"/>
   </bookViews>
@@ -153,9 +153,6 @@
     <t xml:space="preserve">Tên khách hàng </t>
   </si>
   <si>
-    <t>EmployeeName</t>
-  </si>
-  <si>
     <t>Số điện thoại</t>
   </si>
   <si>
@@ -343,6 +340,9 @@
   </si>
   <si>
     <t>Người sửa</t>
+  </si>
+  <si>
+    <t>CustomerName</t>
   </si>
 </sst>
 </file>
@@ -782,8 +782,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F93C9DBF-709E-4039-B299-89A574944C00}">
   <dimension ref="A3:Q43"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C4" sqref="C4:F5"/>
+    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="G23" sqref="G23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -793,10 +793,10 @@
     <col min="3" max="3" width="17.140625" customWidth="1"/>
     <col min="4" max="5" width="14.42578125" customWidth="1"/>
     <col min="6" max="6" width="21.140625" customWidth="1"/>
-    <col min="7" max="7" width="15.5703125" customWidth="1"/>
-    <col min="8" max="8" width="14.42578125" customWidth="1"/>
-    <col min="9" max="9" width="14.7109375" customWidth="1"/>
-    <col min="10" max="10" width="19.7109375" customWidth="1"/>
+    <col min="7" max="7" width="22.7109375" customWidth="1"/>
+    <col min="8" max="8" width="23.85546875" customWidth="1"/>
+    <col min="9" max="9" width="19.28515625" customWidth="1"/>
+    <col min="10" max="10" width="25.28515625" customWidth="1"/>
     <col min="11" max="11" width="20.28515625" customWidth="1"/>
     <col min="12" max="12" width="21.7109375" customWidth="1"/>
     <col min="13" max="13" width="28.7109375" customWidth="1"/>
@@ -811,7 +811,7 @@
         <v>0</v>
       </c>
       <c r="B3" s="10" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.25">
@@ -822,16 +822,16 @@
         <v>2</v>
       </c>
       <c r="C4" s="1" t="s">
+        <v>98</v>
+      </c>
+      <c r="D4" s="1" t="s">
         <v>99</v>
       </c>
-      <c r="D4" s="1" t="s">
-        <v>100</v>
-      </c>
       <c r="E4" s="1" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="F4" s="1" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.25">
@@ -842,16 +842,16 @@
         <v>4</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="D5" s="1" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="E5" s="1" t="s">
+        <v>102</v>
+      </c>
+      <c r="F5" s="1" t="s">
         <v>103</v>
-      </c>
-      <c r="F5" s="1" t="s">
-        <v>104</v>
       </c>
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.25">
@@ -859,7 +859,7 @@
         <v>20</v>
       </c>
       <c r="B8" s="9" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
     </row>
     <row r="9" spans="1:9" x14ac:dyDescent="0.25">
@@ -870,25 +870,25 @@
         <v>25</v>
       </c>
       <c r="C9" s="1" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="D9" s="1" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="E9" s="1" t="s">
         <v>20</v>
       </c>
       <c r="F9" s="1" t="s">
+        <v>98</v>
+      </c>
+      <c r="G9" s="1" t="s">
         <v>99</v>
       </c>
-      <c r="G9" s="1" t="s">
-        <v>100</v>
-      </c>
       <c r="H9" s="1" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="I9" s="1" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
     </row>
     <row r="10" spans="1:9" x14ac:dyDescent="0.25">
@@ -899,30 +899,30 @@
         <v>29</v>
       </c>
       <c r="C10" s="1" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="D10" s="1" t="s">
+        <v>94</v>
+      </c>
+      <c r="E10" s="1" t="s">
         <v>95</v>
       </c>
-      <c r="E10" s="1" t="s">
-        <v>96</v>
-      </c>
       <c r="F10" s="1" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="G10" s="1" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="H10" s="1" t="s">
+        <v>102</v>
+      </c>
+      <c r="I10" s="1" t="s">
         <v>103</v>
-      </c>
-      <c r="I10" s="1" t="s">
-        <v>104</v>
       </c>
     </row>
     <row r="11" spans="1:9" x14ac:dyDescent="0.25">
       <c r="E11" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
     </row>
     <row r="12" spans="1:9" x14ac:dyDescent="0.25">
@@ -930,7 +930,7 @@
         <v>19</v>
       </c>
       <c r="B12" s="9" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
     </row>
     <row r="13" spans="1:9" x14ac:dyDescent="0.25">
@@ -941,16 +941,16 @@
         <v>31</v>
       </c>
       <c r="C13" s="1" t="s">
+        <v>98</v>
+      </c>
+      <c r="D13" s="1" t="s">
         <v>99</v>
       </c>
-      <c r="D13" s="1" t="s">
-        <v>100</v>
-      </c>
       <c r="E13" s="1" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="F13" s="1" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
     </row>
     <row r="14" spans="1:9" x14ac:dyDescent="0.25">
@@ -961,64 +961,64 @@
         <v>35</v>
       </c>
       <c r="C14" s="1" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="D14" s="1" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="E14" s="1" t="s">
+        <v>102</v>
+      </c>
+      <c r="F14" s="1" t="s">
         <v>103</v>
-      </c>
-      <c r="F14" s="1" t="s">
-        <v>104</v>
       </c>
     </row>
     <row r="16" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A16" s="7" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="B16" s="11" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
     </row>
     <row r="17" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A17" s="1" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="B17" s="1" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="C17" s="1" t="s">
+        <v>98</v>
+      </c>
+      <c r="D17" s="1" t="s">
         <v>99</v>
       </c>
-      <c r="D17" s="1" t="s">
-        <v>100</v>
-      </c>
       <c r="E17" s="1" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="F17" s="1" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
     </row>
     <row r="18" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A18" s="1" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="B18" s="1" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="C18" s="1" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="D18" s="1" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="E18" s="1" t="s">
+        <v>102</v>
+      </c>
+      <c r="F18" s="1" t="s">
         <v>103</v>
-      </c>
-      <c r="F18" s="1" t="s">
-        <v>104</v>
       </c>
     </row>
     <row r="21" spans="1:17" x14ac:dyDescent="0.25">
@@ -1026,7 +1026,7 @@
         <v>36</v>
       </c>
       <c r="B21" s="9" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
     </row>
     <row r="22" spans="1:17" x14ac:dyDescent="0.25">
@@ -1040,46 +1040,46 @@
         <v>41</v>
       </c>
       <c r="D22" s="1" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="E22" s="1" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="F22" s="1" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="G22" s="1" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="H22" s="1" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="I22" s="1" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="J22" s="1" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="K22" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="L22" s="1" t="s">
         <v>59</v>
       </c>
-      <c r="L22" s="1" t="s">
-        <v>60</v>
-      </c>
       <c r="M22" s="1" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="N22" s="1" t="s">
+        <v>98</v>
+      </c>
+      <c r="O22" s="1" t="s">
         <v>99</v>
       </c>
-      <c r="O22" s="1" t="s">
-        <v>100</v>
-      </c>
       <c r="P22" s="1" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="Q22" s="1" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
     </row>
     <row r="23" spans="1:17" x14ac:dyDescent="0.25">
@@ -1090,210 +1090,210 @@
         <v>40</v>
       </c>
       <c r="C23" s="1" t="s">
-        <v>42</v>
+        <v>105</v>
       </c>
       <c r="D23" s="1" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="E23" s="1" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="F23" s="1" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="G23" s="1" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="H23" s="1" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="I23" s="1" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="J23" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="K23" s="1" t="s">
         <v>57</v>
       </c>
-      <c r="K23" s="1" t="s">
-        <v>58</v>
-      </c>
       <c r="L23" s="1" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="M23" s="1" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="N23" s="1" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="O23" s="1" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="P23" s="1" t="s">
+        <v>102</v>
+      </c>
+      <c r="Q23" s="1" t="s">
         <v>103</v>
-      </c>
-      <c r="Q23" s="1" t="s">
-        <v>104</v>
       </c>
     </row>
     <row r="24" spans="1:17" x14ac:dyDescent="0.25">
       <c r="G24" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
     </row>
     <row r="27" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A27" s="8" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="B27" s="9" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
     </row>
     <row r="28" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A28" s="1" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="B28" s="1" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="C28" s="1" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="D28" s="1" t="s">
+        <v>98</v>
+      </c>
+      <c r="E28" s="1" t="s">
         <v>99</v>
       </c>
-      <c r="E28" s="1" t="s">
-        <v>100</v>
-      </c>
       <c r="F28" s="1" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="G28" s="1" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
     </row>
     <row r="29" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A29" s="1" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="B29" s="1" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="C29" s="1" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="D29" s="1" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="E29" s="1" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="F29" s="1" t="s">
+        <v>102</v>
+      </c>
+      <c r="G29" s="1" t="s">
         <v>103</v>
-      </c>
-      <c r="G29" s="1" t="s">
-        <v>104</v>
       </c>
     </row>
     <row r="31" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A31" s="8" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="B31" s="9" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
     </row>
     <row r="32" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A32" s="1" t="s">
+        <v>73</v>
+      </c>
+      <c r="B32" s="1" t="s">
         <v>74</v>
       </c>
-      <c r="B32" s="1" t="s">
+      <c r="C32" s="1" t="s">
         <v>75</v>
       </c>
-      <c r="C32" s="1" t="s">
-        <v>76</v>
-      </c>
       <c r="D32" s="1" t="s">
+        <v>98</v>
+      </c>
+      <c r="E32" s="1" t="s">
         <v>99</v>
       </c>
-      <c r="E32" s="1" t="s">
-        <v>100</v>
-      </c>
       <c r="F32" s="1" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="G32" s="1" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
     </row>
     <row r="33" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A33" s="1" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="B33" s="1" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="C33" s="1" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="D33" s="1" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="E33" s="1" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="F33" s="1" t="s">
+        <v>102</v>
+      </c>
+      <c r="G33" s="1" t="s">
         <v>103</v>
-      </c>
-      <c r="G33" s="1" t="s">
-        <v>104</v>
       </c>
     </row>
     <row r="35" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A35" s="8" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="B35" s="9" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
     </row>
     <row r="36" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A36" s="1" t="s">
+        <v>78</v>
+      </c>
+      <c r="B36" s="1" t="s">
         <v>79</v>
       </c>
-      <c r="B36" s="1" t="s">
-        <v>80</v>
-      </c>
       <c r="C36" s="1" t="s">
+        <v>98</v>
+      </c>
+      <c r="D36" s="1" t="s">
         <v>99</v>
       </c>
-      <c r="D36" s="1" t="s">
-        <v>100</v>
-      </c>
       <c r="E36" s="1" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="F36" s="1" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
     </row>
     <row r="37" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A37" s="1" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="B37" s="1" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="C37" s="1" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="D37" s="1" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="E37" s="1" t="s">
+        <v>102</v>
+      </c>
+      <c r="F37" s="1" t="s">
         <v>103</v>
-      </c>
-      <c r="F37" s="1" t="s">
-        <v>104</v>
       </c>
     </row>
     <row r="39" spans="1:16" x14ac:dyDescent="0.25">
@@ -1301,15 +1301,15 @@
         <v>5</v>
       </c>
       <c r="B39" s="9" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
     </row>
     <row r="40" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A40" s="1" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="B40" s="1" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="C40" s="1" t="s">
         <v>21</v>
@@ -1342,16 +1342,16 @@
         <v>25</v>
       </c>
       <c r="M40" s="1" t="s">
+        <v>98</v>
+      </c>
+      <c r="N40" s="1" t="s">
         <v>99</v>
       </c>
-      <c r="N40" s="1" t="s">
-        <v>100</v>
-      </c>
       <c r="O40" s="1" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="P40" s="1" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
     </row>
     <row r="41" spans="1:16" x14ac:dyDescent="0.25">
@@ -1392,16 +1392,16 @@
         <v>27</v>
       </c>
       <c r="M41" s="1" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="N41" s="1" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="O41" s="1" t="s">
+        <v>102</v>
+      </c>
+      <c r="P41" s="1" t="s">
         <v>103</v>
-      </c>
-      <c r="P41" s="1" t="s">
-        <v>104</v>
       </c>
     </row>
     <row r="42" spans="1:16" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Thêm chức năng thêm đơn hàng
</commit_message>
<xml_diff>
--- a/ldtiep.docs/Cấu trúc bảng.xlsx
+++ b/ldtiep.docs/Cấu trúc bảng.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\do-an\ldtiep.docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CF97C67D-B131-4EC6-8107-3837FB4F59F8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C1200CB9-C913-4828-9041-4D7DB39F65F7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{2010E0CC-8981-4F39-BFC2-E9E2B2601EEF}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="182" uniqueCount="106">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="180" uniqueCount="107">
   <si>
     <t>Bảng lưu màu sắc</t>
   </si>
@@ -165,12 +165,6 @@
     <t>Email</t>
   </si>
   <si>
-    <t>Hình thức vận chuyển</t>
-  </si>
-  <si>
-    <t>TransType</t>
-  </si>
-  <si>
     <t xml:space="preserve">Địa chỉ khách hàng </t>
   </si>
   <si>
@@ -192,12 +186,6 @@
     <t>EmployeeNote</t>
   </si>
   <si>
-    <t>Phương thức vận chuyển</t>
-  </si>
-  <si>
-    <t>TransSpeed</t>
-  </si>
-  <si>
     <t>TransCost</t>
   </si>
   <si>
@@ -207,9 +195,6 @@
     <t>Phương thức thanh toán</t>
   </si>
   <si>
-    <t>PaymentType</t>
-  </si>
-  <si>
     <t>Tên phương thức thanh toán</t>
   </si>
   <si>
@@ -343,13 +328,31 @@
   </si>
   <si>
     <t>CustomerName</t>
+  </si>
+  <si>
+    <t>Giảm giá vận chuyển</t>
+  </si>
+  <si>
+    <t>Tổng giá trị sản phẩm</t>
+  </si>
+  <si>
+    <t>Tổng thanh toán</t>
+  </si>
+  <si>
+    <t>TotalPrice</t>
+  </si>
+  <si>
+    <t>TransCostDiscount</t>
+  </si>
+  <si>
+    <t>TotalPay</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -372,6 +375,24 @@
       <family val="2"/>
       <charset val="163"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FF616161"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="15"/>
+      <color rgb="FF1C2430"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFABB2BF"/>
+      <name val="Consolas"/>
+      <family val="3"/>
     </font>
   </fonts>
   <fills count="9">
@@ -451,7 +472,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="16">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
@@ -466,6 +487,12 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="2" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -780,10 +807,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F93C9DBF-709E-4039-B299-89A574944C00}">
-  <dimension ref="A3:Q43"/>
+  <dimension ref="A3:P43"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="G23" sqref="G23"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="H17" sqref="H17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -795,9 +822,9 @@
     <col min="6" max="6" width="21.140625" customWidth="1"/>
     <col min="7" max="7" width="22.7109375" customWidth="1"/>
     <col min="8" max="8" width="23.85546875" customWidth="1"/>
-    <col min="9" max="9" width="19.28515625" customWidth="1"/>
+    <col min="9" max="9" width="25.5703125" customWidth="1"/>
     <col min="10" max="10" width="25.28515625" customWidth="1"/>
-    <col min="11" max="11" width="20.28515625" customWidth="1"/>
+    <col min="11" max="11" width="25.42578125" customWidth="1"/>
     <col min="12" max="12" width="21.7109375" customWidth="1"/>
     <col min="13" max="13" width="28.7109375" customWidth="1"/>
     <col min="14" max="14" width="23.140625" customWidth="1"/>
@@ -811,7 +838,7 @@
         <v>0</v>
       </c>
       <c r="B3" s="10" t="s">
-        <v>85</v>
+        <v>80</v>
       </c>
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.25">
@@ -822,16 +849,16 @@
         <v>2</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>98</v>
+        <v>93</v>
       </c>
       <c r="D4" s="1" t="s">
+        <v>94</v>
+      </c>
+      <c r="E4" s="1" t="s">
+        <v>96</v>
+      </c>
+      <c r="F4" s="1" t="s">
         <v>99</v>
-      </c>
-      <c r="E4" s="1" t="s">
-        <v>101</v>
-      </c>
-      <c r="F4" s="1" t="s">
-        <v>104</v>
       </c>
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.25">
@@ -842,16 +869,16 @@
         <v>4</v>
       </c>
       <c r="C5" s="1" t="s">
+        <v>92</v>
+      </c>
+      <c r="D5" s="1" t="s">
+        <v>95</v>
+      </c>
+      <c r="E5" s="1" t="s">
         <v>97</v>
       </c>
-      <c r="D5" s="1" t="s">
-        <v>100</v>
-      </c>
-      <c r="E5" s="1" t="s">
-        <v>102</v>
-      </c>
       <c r="F5" s="1" t="s">
-        <v>103</v>
+        <v>98</v>
       </c>
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.25">
@@ -859,7 +886,7 @@
         <v>20</v>
       </c>
       <c r="B8" s="9" t="s">
-        <v>86</v>
+        <v>81</v>
       </c>
     </row>
     <row r="9" spans="1:9" x14ac:dyDescent="0.25">
@@ -870,25 +897,25 @@
         <v>25</v>
       </c>
       <c r="C9" s="1" t="s">
-        <v>91</v>
+        <v>86</v>
       </c>
       <c r="D9" s="1" t="s">
-        <v>93</v>
+        <v>88</v>
       </c>
       <c r="E9" s="1" t="s">
         <v>20</v>
       </c>
       <c r="F9" s="1" t="s">
-        <v>98</v>
+        <v>93</v>
       </c>
       <c r="G9" s="1" t="s">
+        <v>94</v>
+      </c>
+      <c r="H9" s="1" t="s">
+        <v>96</v>
+      </c>
+      <c r="I9" s="1" t="s">
         <v>99</v>
-      </c>
-      <c r="H9" s="1" t="s">
-        <v>101</v>
-      </c>
-      <c r="I9" s="1" t="s">
-        <v>104</v>
       </c>
     </row>
     <row r="10" spans="1:9" x14ac:dyDescent="0.25">
@@ -899,30 +926,30 @@
         <v>29</v>
       </c>
       <c r="C10" s="1" t="s">
+        <v>87</v>
+      </c>
+      <c r="D10" s="1" t="s">
+        <v>89</v>
+      </c>
+      <c r="E10" s="1" t="s">
+        <v>90</v>
+      </c>
+      <c r="F10" s="1" t="s">
         <v>92</v>
       </c>
-      <c r="D10" s="1" t="s">
-        <v>94</v>
-      </c>
-      <c r="E10" s="1" t="s">
+      <c r="G10" s="1" t="s">
         <v>95</v>
       </c>
-      <c r="F10" s="1" t="s">
+      <c r="H10" s="1" t="s">
         <v>97</v>
       </c>
-      <c r="G10" s="1" t="s">
-        <v>100</v>
-      </c>
-      <c r="H10" s="1" t="s">
-        <v>102</v>
-      </c>
       <c r="I10" s="1" t="s">
-        <v>103</v>
+        <v>98</v>
       </c>
     </row>
     <row r="11" spans="1:9" x14ac:dyDescent="0.25">
       <c r="E11" t="s">
-        <v>96</v>
+        <v>91</v>
       </c>
     </row>
     <row r="12" spans="1:9" x14ac:dyDescent="0.25">
@@ -930,7 +957,7 @@
         <v>19</v>
       </c>
       <c r="B12" s="9" t="s">
-        <v>87</v>
+        <v>82</v>
       </c>
     </row>
     <row r="13" spans="1:9" x14ac:dyDescent="0.25">
@@ -941,16 +968,16 @@
         <v>31</v>
       </c>
       <c r="C13" s="1" t="s">
-        <v>98</v>
+        <v>93</v>
       </c>
       <c r="D13" s="1" t="s">
+        <v>94</v>
+      </c>
+      <c r="E13" s="1" t="s">
+        <v>96</v>
+      </c>
+      <c r="F13" s="1" t="s">
         <v>99</v>
-      </c>
-      <c r="E13" s="1" t="s">
-        <v>101</v>
-      </c>
-      <c r="F13" s="1" t="s">
-        <v>104</v>
       </c>
     </row>
     <row r="14" spans="1:9" x14ac:dyDescent="0.25">
@@ -961,75 +988,75 @@
         <v>35</v>
       </c>
       <c r="C14" s="1" t="s">
+        <v>92</v>
+      </c>
+      <c r="D14" s="1" t="s">
+        <v>95</v>
+      </c>
+      <c r="E14" s="1" t="s">
         <v>97</v>
       </c>
-      <c r="D14" s="1" t="s">
-        <v>100</v>
-      </c>
-      <c r="E14" s="1" t="s">
-        <v>102</v>
-      </c>
       <c r="F14" s="1" t="s">
-        <v>103</v>
+        <v>98</v>
       </c>
     </row>
     <row r="16" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A16" s="7" t="s">
+        <v>55</v>
+      </c>
+      <c r="B16" s="11" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="17" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A17" s="1" t="s">
         <v>59</v>
       </c>
-      <c r="B16" s="11" t="s">
-        <v>88</v>
-      </c>
-    </row>
-    <row r="17" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A17" s="1" t="s">
-        <v>64</v>
-      </c>
       <c r="B17" s="1" t="s">
-        <v>61</v>
+        <v>56</v>
       </c>
       <c r="C17" s="1" t="s">
+        <v>93</v>
+      </c>
+      <c r="D17" s="1" t="s">
+        <v>94</v>
+      </c>
+      <c r="E17" s="1" t="s">
+        <v>96</v>
+      </c>
+      <c r="F17" s="1" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="18" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A18" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="B18" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="C18" s="1" t="s">
+        <v>92</v>
+      </c>
+      <c r="D18" s="1" t="s">
+        <v>95</v>
+      </c>
+      <c r="E18" s="1" t="s">
+        <v>97</v>
+      </c>
+      <c r="F18" s="1" t="s">
         <v>98</v>
       </c>
-      <c r="D17" s="1" t="s">
-        <v>99</v>
-      </c>
-      <c r="E17" s="1" t="s">
-        <v>101</v>
-      </c>
-      <c r="F17" s="1" t="s">
-        <v>104</v>
-      </c>
-    </row>
-    <row r="18" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A18" s="1" t="s">
-        <v>63</v>
-      </c>
-      <c r="B18" s="1" t="s">
-        <v>62</v>
-      </c>
-      <c r="C18" s="1" t="s">
-        <v>97</v>
-      </c>
-      <c r="D18" s="1" t="s">
-        <v>100</v>
-      </c>
-      <c r="E18" s="1" t="s">
-        <v>102</v>
-      </c>
-      <c r="F18" s="1" t="s">
-        <v>103</v>
-      </c>
-    </row>
-    <row r="21" spans="1:17" x14ac:dyDescent="0.25">
+    </row>
+    <row r="21" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A21" s="5" t="s">
         <v>36</v>
       </c>
       <c r="B21" s="9" t="s">
-        <v>80</v>
-      </c>
-    </row>
-    <row r="22" spans="1:17" x14ac:dyDescent="0.25">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="22" spans="1:16" ht="18.75" x14ac:dyDescent="0.25">
       <c r="A22" s="1" t="s">
         <v>37</v>
       </c>
@@ -1049,40 +1076,37 @@
         <v>46</v>
       </c>
       <c r="G22" s="1" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="H22" s="1" t="s">
         <v>51</v>
       </c>
       <c r="I22" s="1" t="s">
-        <v>53</v>
-      </c>
-      <c r="J22" s="1" t="s">
-        <v>55</v>
-      </c>
-      <c r="K22" s="1" t="s">
-        <v>58</v>
-      </c>
-      <c r="L22" s="1" t="s">
-        <v>59</v>
+        <v>54</v>
+      </c>
+      <c r="J22" s="12" t="s">
+        <v>101</v>
+      </c>
+      <c r="K22" s="13" t="s">
+        <v>102</v>
+      </c>
+      <c r="L22" s="14" t="s">
+        <v>103</v>
       </c>
       <c r="M22" s="1" t="s">
-        <v>61</v>
+        <v>93</v>
       </c>
       <c r="N22" s="1" t="s">
-        <v>98</v>
+        <v>94</v>
       </c>
       <c r="O22" s="1" t="s">
+        <v>96</v>
+      </c>
+      <c r="P22" s="1" t="s">
         <v>99</v>
       </c>
-      <c r="P22" s="1" t="s">
-        <v>101</v>
-      </c>
-      <c r="Q22" s="1" t="s">
-        <v>104</v>
-      </c>
-    </row>
-    <row r="23" spans="1:17" x14ac:dyDescent="0.25">
+    </row>
+    <row r="23" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A23" s="1" t="s">
         <v>39</v>
       </c>
@@ -1090,7 +1114,7 @@
         <v>40</v>
       </c>
       <c r="C23" s="1" t="s">
-        <v>105</v>
+        <v>100</v>
       </c>
       <c r="D23" s="1" t="s">
         <v>43</v>
@@ -1102,198 +1126,195 @@
         <v>47</v>
       </c>
       <c r="G23" s="1" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="H23" s="1" t="s">
         <v>52</v>
       </c>
-      <c r="I23" s="1" t="s">
-        <v>54</v>
-      </c>
-      <c r="J23" s="1" t="s">
-        <v>56</v>
-      </c>
-      <c r="K23" s="1" t="s">
-        <v>57</v>
-      </c>
-      <c r="L23" s="1" t="s">
-        <v>60</v>
+      <c r="I23" s="15" t="s">
+        <v>53</v>
+      </c>
+      <c r="J23" s="15" t="s">
+        <v>105</v>
+      </c>
+      <c r="K23" s="15" t="s">
+        <v>106</v>
+      </c>
+      <c r="L23" s="15" t="s">
+        <v>104</v>
       </c>
       <c r="M23" s="1" t="s">
+        <v>92</v>
+      </c>
+      <c r="N23" s="1" t="s">
+        <v>95</v>
+      </c>
+      <c r="O23" s="1" t="s">
+        <v>97</v>
+      </c>
+      <c r="P23" s="1" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="24" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="F24" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="27" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A27" s="8" t="s">
+        <v>61</v>
+      </c>
+      <c r="B27" s="9" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="28" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A28" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="B28" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="C28" s="1" t="s">
+        <v>72</v>
+      </c>
+      <c r="D28" s="1" t="s">
+        <v>93</v>
+      </c>
+      <c r="E28" s="1" t="s">
+        <v>94</v>
+      </c>
+      <c r="F28" s="1" t="s">
+        <v>96</v>
+      </c>
+      <c r="G28" s="1" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="29" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A29" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="B29" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="C29" s="1" t="s">
+        <v>71</v>
+      </c>
+      <c r="D29" s="1" t="s">
+        <v>92</v>
+      </c>
+      <c r="E29" s="1" t="s">
+        <v>95</v>
+      </c>
+      <c r="F29" s="1" t="s">
+        <v>97</v>
+      </c>
+      <c r="G29" s="1" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="31" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A31" s="8" t="s">
         <v>62</v>
       </c>
-      <c r="N23" s="1" t="s">
-        <v>97</v>
-      </c>
-      <c r="O23" s="1" t="s">
-        <v>100</v>
-      </c>
-      <c r="P23" s="1" t="s">
-        <v>102</v>
-      </c>
-      <c r="Q23" s="1" t="s">
-        <v>103</v>
-      </c>
-    </row>
-    <row r="24" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="G24" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="27" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A27" s="8" t="s">
-        <v>66</v>
-      </c>
-      <c r="B27" s="9" t="s">
-        <v>81</v>
-      </c>
-    </row>
-    <row r="28" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A28" s="1" t="s">
+      <c r="B31" s="9" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="32" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A32" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="B32" s="1" t="s">
         <v>69</v>
       </c>
-      <c r="B28" s="1" t="s">
-        <v>72</v>
-      </c>
-      <c r="C28" s="1" t="s">
-        <v>77</v>
-      </c>
-      <c r="D28" s="1" t="s">
-        <v>98</v>
-      </c>
-      <c r="E28" s="1" t="s">
+      <c r="C32" s="1" t="s">
+        <v>70</v>
+      </c>
+      <c r="D32" s="1" t="s">
+        <v>93</v>
+      </c>
+      <c r="E32" s="1" t="s">
+        <v>94</v>
+      </c>
+      <c r="F32" s="1" t="s">
+        <v>96</v>
+      </c>
+      <c r="G32" s="1" t="s">
         <v>99</v>
-      </c>
-      <c r="F28" s="1" t="s">
-        <v>101</v>
-      </c>
-      <c r="G28" s="1" t="s">
-        <v>104</v>
-      </c>
-    </row>
-    <row r="29" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A29" s="1" t="s">
-        <v>68</v>
-      </c>
-      <c r="B29" s="1" t="s">
-        <v>70</v>
-      </c>
-      <c r="C29" s="1" t="s">
-        <v>76</v>
-      </c>
-      <c r="D29" s="1" t="s">
-        <v>97</v>
-      </c>
-      <c r="E29" s="1" t="s">
-        <v>100</v>
-      </c>
-      <c r="F29" s="1" t="s">
-        <v>102</v>
-      </c>
-      <c r="G29" s="1" t="s">
-        <v>103</v>
-      </c>
-    </row>
-    <row r="31" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A31" s="8" t="s">
-        <v>67</v>
-      </c>
-      <c r="B31" s="9" t="s">
-        <v>82</v>
-      </c>
-    </row>
-    <row r="32" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A32" s="1" t="s">
-        <v>73</v>
-      </c>
-      <c r="B32" s="1" t="s">
-        <v>74</v>
-      </c>
-      <c r="C32" s="1" t="s">
-        <v>75</v>
-      </c>
-      <c r="D32" s="1" t="s">
-        <v>98</v>
-      </c>
-      <c r="E32" s="1" t="s">
-        <v>99</v>
-      </c>
-      <c r="F32" s="1" t="s">
-        <v>101</v>
-      </c>
-      <c r="G32" s="1" t="s">
-        <v>104</v>
       </c>
     </row>
     <row r="33" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A33" s="1" t="s">
-        <v>71</v>
+        <v>66</v>
       </c>
       <c r="B33" s="1" t="s">
-        <v>70</v>
+        <v>65</v>
       </c>
       <c r="C33" s="1" t="s">
-        <v>68</v>
+        <v>63</v>
       </c>
       <c r="D33" s="1" t="s">
+        <v>92</v>
+      </c>
+      <c r="E33" s="1" t="s">
+        <v>95</v>
+      </c>
+      <c r="F33" s="1" t="s">
         <v>97</v>
       </c>
-      <c r="E33" s="1" t="s">
-        <v>100</v>
-      </c>
-      <c r="F33" s="1" t="s">
-        <v>102</v>
-      </c>
       <c r="G33" s="1" t="s">
-        <v>103</v>
+        <v>98</v>
       </c>
     </row>
     <row r="35" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A35" s="8" t="s">
-        <v>65</v>
+        <v>60</v>
       </c>
       <c r="B35" s="9" t="s">
-        <v>83</v>
+        <v>78</v>
       </c>
     </row>
     <row r="36" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A36" s="1" t="s">
-        <v>78</v>
+        <v>73</v>
       </c>
       <c r="B36" s="1" t="s">
-        <v>79</v>
+        <v>74</v>
       </c>
       <c r="C36" s="1" t="s">
-        <v>98</v>
+        <v>93</v>
       </c>
       <c r="D36" s="1" t="s">
+        <v>94</v>
+      </c>
+      <c r="E36" s="1" t="s">
+        <v>96</v>
+      </c>
+      <c r="F36" s="1" t="s">
         <v>99</v>
-      </c>
-      <c r="E36" s="1" t="s">
-        <v>101</v>
-      </c>
-      <c r="F36" s="1" t="s">
-        <v>104</v>
       </c>
     </row>
     <row r="37" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A37" s="1" t="s">
-        <v>76</v>
+        <v>71</v>
       </c>
       <c r="B37" s="1" t="s">
-        <v>70</v>
+        <v>65</v>
       </c>
       <c r="C37" s="1" t="s">
+        <v>92</v>
+      </c>
+      <c r="D37" s="1" t="s">
+        <v>95</v>
+      </c>
+      <c r="E37" s="1" t="s">
         <v>97</v>
       </c>
-      <c r="D37" s="1" t="s">
-        <v>100</v>
-      </c>
-      <c r="E37" s="1" t="s">
-        <v>102</v>
-      </c>
       <c r="F37" s="1" t="s">
-        <v>103</v>
+        <v>98</v>
       </c>
     </row>
     <row r="39" spans="1:16" x14ac:dyDescent="0.25">
@@ -1301,15 +1322,15 @@
         <v>5</v>
       </c>
       <c r="B39" s="9" t="s">
-        <v>84</v>
+        <v>79</v>
       </c>
     </row>
     <row r="40" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A40" s="1" t="s">
-        <v>90</v>
+        <v>85</v>
       </c>
       <c r="B40" s="1" t="s">
-        <v>89</v>
+        <v>84</v>
       </c>
       <c r="C40" s="1" t="s">
         <v>21</v>
@@ -1342,16 +1363,16 @@
         <v>25</v>
       </c>
       <c r="M40" s="1" t="s">
-        <v>98</v>
+        <v>93</v>
       </c>
       <c r="N40" s="1" t="s">
+        <v>94</v>
+      </c>
+      <c r="O40" s="1" t="s">
+        <v>96</v>
+      </c>
+      <c r="P40" s="1" t="s">
         <v>99</v>
-      </c>
-      <c r="O40" s="1" t="s">
-        <v>101</v>
-      </c>
-      <c r="P40" s="1" t="s">
-        <v>104</v>
       </c>
     </row>
     <row r="41" spans="1:16" x14ac:dyDescent="0.25">
@@ -1392,16 +1413,16 @@
         <v>27</v>
       </c>
       <c r="M41" s="1" t="s">
+        <v>92</v>
+      </c>
+      <c r="N41" s="1" t="s">
+        <v>95</v>
+      </c>
+      <c r="O41" s="1" t="s">
         <v>97</v>
       </c>
-      <c r="N41" s="1" t="s">
-        <v>100</v>
-      </c>
-      <c r="O41" s="1" t="s">
-        <v>102</v>
-      </c>
       <c r="P41" s="1" t="s">
-        <v>103</v>
+        <v>98</v>
       </c>
     </row>
     <row r="42" spans="1:16" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Thêm phân hệ nhân viên và vẽ màn phân quyền
</commit_message>
<xml_diff>
--- a/ldtiep.docs/Cấu trúc bảng.xlsx
+++ b/ldtiep.docs/Cấu trúc bảng.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\do-an\ldtiep.docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C1200CB9-C913-4828-9041-4D7DB39F65F7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{35DB7FFF-FADA-4F80-AC20-E3A4D266596D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{2010E0CC-8981-4F39-BFC2-E9E2B2601EEF}"/>
+    <workbookView xWindow="4695" yWindow="615" windowWidth="24105" windowHeight="11295" xr2:uid="{2010E0CC-8981-4F39-BFC2-E9E2B2601EEF}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="180" uniqueCount="107">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="196" uniqueCount="122">
   <si>
     <t>Bảng lưu màu sắc</t>
   </si>
@@ -346,6 +346,51 @@
   </si>
   <si>
     <t>TotalPay</t>
+  </si>
+  <si>
+    <t>Nhân viên</t>
+  </si>
+  <si>
+    <t>ldt_employee</t>
+  </si>
+  <si>
+    <t>EmployeeID</t>
+  </si>
+  <si>
+    <t>ID Nhân viên</t>
+  </si>
+  <si>
+    <t>Tên nhân viên</t>
+  </si>
+  <si>
+    <t>EmployeeName</t>
+  </si>
+  <si>
+    <t>EmployeeCode</t>
+  </si>
+  <si>
+    <t>Mã nhân viên</t>
+  </si>
+  <si>
+    <t>Quyền</t>
+  </si>
+  <si>
+    <t>Rules</t>
+  </si>
+  <si>
+    <t>ID quyền</t>
+  </si>
+  <si>
+    <t>Tên quyền</t>
+  </si>
+  <si>
+    <t>RuleID</t>
+  </si>
+  <si>
+    <t>RuleName</t>
+  </si>
+  <si>
+    <t>ldt_rule</t>
   </si>
 </sst>
 </file>
@@ -487,12 +532,12 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="2" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -807,10 +852,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F93C9DBF-709E-4039-B299-89A574944C00}">
-  <dimension ref="A3:P43"/>
+  <dimension ref="A3:P50"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H17" sqref="H17"/>
+    <sheetView tabSelected="1" topLeftCell="A37" workbookViewId="0">
+      <selection activeCell="D46" sqref="D46"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1084,13 +1129,13 @@
       <c r="I22" s="1" t="s">
         <v>54</v>
       </c>
-      <c r="J22" s="12" t="s">
+      <c r="J22" s="1" t="s">
         <v>101</v>
       </c>
-      <c r="K22" s="13" t="s">
+      <c r="K22" s="12" t="s">
         <v>102</v>
       </c>
-      <c r="L22" s="14" t="s">
+      <c r="L22" s="13" t="s">
         <v>103</v>
       </c>
       <c r="M22" s="1" t="s">
@@ -1131,16 +1176,16 @@
       <c r="H23" s="1" t="s">
         <v>52</v>
       </c>
-      <c r="I23" s="15" t="s">
+      <c r="I23" s="14" t="s">
         <v>53</v>
       </c>
-      <c r="J23" s="15" t="s">
+      <c r="J23" s="14" t="s">
         <v>105</v>
       </c>
-      <c r="K23" s="15" t="s">
+      <c r="K23" s="14" t="s">
         <v>106</v>
       </c>
-      <c r="L23" s="15" t="s">
+      <c r="L23" s="14" t="s">
         <v>104</v>
       </c>
       <c r="M23" s="1" t="s">
@@ -1433,6 +1478,66 @@
     <row r="43" spans="1:16" x14ac:dyDescent="0.25">
       <c r="C43" t="s">
         <v>10</v>
+      </c>
+    </row>
+    <row r="44" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A44" s="15" t="s">
+        <v>107</v>
+      </c>
+      <c r="B44" s="9" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="45" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A45" s="1" t="s">
+        <v>110</v>
+      </c>
+      <c r="B45" s="1" t="s">
+        <v>111</v>
+      </c>
+      <c r="C45" s="1" t="s">
+        <v>114</v>
+      </c>
+      <c r="D45" s="1" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="46" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A46" s="1" t="s">
+        <v>109</v>
+      </c>
+      <c r="B46" s="1" t="s">
+        <v>112</v>
+      </c>
+      <c r="C46" s="1" t="s">
+        <v>113</v>
+      </c>
+      <c r="D46" s="1" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="48" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A48" s="4" t="s">
+        <v>115</v>
+      </c>
+      <c r="B48" s="9" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="49" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A49" s="1" t="s">
+        <v>117</v>
+      </c>
+      <c r="B49" s="1" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="50" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A50" s="1" t="s">
+        <v>119</v>
+      </c>
+      <c r="B50" s="1" t="s">
+        <v>120</v>
       </c>
     </row>
   </sheetData>

</xml_diff>